<commit_message>
Add more data fetchers
</commit_message>
<xml_diff>
--- a/WhatTheShop_progress.xlsx
+++ b/WhatTheShop_progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jabil-my.sharepoint.com/personal/ihor_shubin_jabil_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\whattheshop-fetcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{333B5567-7381-4E51-B5B2-2CB46D1E16BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A172C99-84A5-45C0-8CE0-DFA51585139F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE849FFE-3B4B-4CF4-BBA9-3992F464C3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{A165CAB8-4234-4E81-A305-F753D69B9A3E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{A165CAB8-4234-4E81-A305-F753D69B9A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="95">
   <si>
     <t>User</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>72 endpoints</t>
+  </si>
+  <si>
+    <t>return empty</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>// it requires sensor or hardware id. It's not available in the API</t>
   </si>
 </sst>
 </file>
@@ -467,7 +476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -483,6 +492,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D883A3CC-69E9-4B5D-8D31-B2725BBDF0A5}">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,7 +833,7 @@
       </c>
       <c r="C1" s="9">
         <f>AVERAGE(B3,B10,B20,B26,B40,B51,B62,B74,B80,B88,B92,B99,B104,B109)</f>
-        <v>0.40932282003710574</v>
+        <v>0.73726551226551218</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>87</v>
@@ -1253,10 +1268,7 @@
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="14">
-        <f>0/8</f>
-        <v>0</v>
-      </c>
+      <c r="B51" s="14"/>
       <c r="C51" s="11"/>
       <c r="D51" s="14">
         <f>0/8</f>
@@ -1324,10 +1336,7 @@
       <c r="A62" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="14">
-        <f>0/9</f>
-        <v>0</v>
-      </c>
+      <c r="B62" s="14"/>
       <c r="C62" s="11"/>
       <c r="D62" s="14">
         <f>0/9</f>
@@ -1402,8 +1411,8 @@
         <v>7</v>
       </c>
       <c r="B74" s="14">
-        <f>0/3</f>
-        <v>0</v>
+        <f>COUNTIF(B76:B78, "+")/COUNTA(B76:B78)</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="14">
@@ -1420,19 +1429,27 @@
       <c r="A76" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="B76" t="s">
+        <v>88</v>
+      </c>
       <c r="E76" s="4"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="B77" t="s">
+        <v>88</v>
+      </c>
       <c r="E77" s="4"/>
     </row>
     <row r="78" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B78" s="6"/>
+      <c r="B78" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="7"/>
@@ -1443,8 +1460,8 @@
         <v>8</v>
       </c>
       <c r="B80" s="14">
-        <f>0/5</f>
-        <v>0</v>
+        <f>COUNTIF(B82:B86, "+")/COUNTA(B82:B86)</f>
+        <v>0.2</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="14">
@@ -1461,31 +1478,45 @@
       <c r="A82" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="B82" t="s">
+        <v>88</v>
+      </c>
       <c r="E82" s="4"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="B83" t="s">
+        <v>93</v>
+      </c>
       <c r="E83" s="4"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="B84" t="s">
+        <v>93</v>
+      </c>
       <c r="E84" s="4"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="B85" t="s">
+        <v>93</v>
+      </c>
       <c r="E85" s="4"/>
     </row>
     <row r="86" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B86" s="6"/>
+      <c r="B86" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
       <c r="E86" s="7"/>
@@ -1496,7 +1527,7 @@
         <v>9</v>
       </c>
       <c r="B88" s="14">
-        <f>1/1</f>
+        <f>COUNTIF(B90, "+")/COUNTA(B90)</f>
         <v>1</v>
       </c>
       <c r="C88" s="11"/>
@@ -1527,8 +1558,8 @@
         <v>10</v>
       </c>
       <c r="B92" s="14">
-        <f>0/4</f>
-        <v>0</v>
+        <f>COUNTIF(B94:B97, "+")/COUNTA(B94:B97)</f>
+        <v>1</v>
       </c>
       <c r="C92" s="11"/>
       <c r="D92" s="14">
@@ -1545,25 +1576,36 @@
       <c r="A94" s="2" t="s">
         <v>74</v>
       </c>
+      <c r="B94" t="s">
+        <v>88</v>
+      </c>
       <c r="E94" s="4"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="B95" t="s">
+        <v>88</v>
+      </c>
       <c r="E95" s="4"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="B96" t="s">
+        <v>88</v>
+      </c>
       <c r="E96" s="4"/>
     </row>
     <row r="97" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B97" s="6"/>
+      <c r="B97" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
       <c r="E97" s="7"/>
@@ -1574,8 +1616,8 @@
         <v>11</v>
       </c>
       <c r="B99" s="14">
-        <f>0/2</f>
-        <v>0</v>
+        <f>COUNTIF(B101:B102, "+")/COUNTA(B101:B102)</f>
+        <v>1</v>
       </c>
       <c r="C99" s="11"/>
       <c r="D99" s="14">
@@ -1592,13 +1634,18 @@
       <c r="A101" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="B101" t="s">
+        <v>88</v>
+      </c>
       <c r="E101" s="4"/>
     </row>
     <row r="102" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B102" s="6"/>
+      <c r="B102" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
       <c r="E102" s="7"/>
@@ -1649,8 +1696,8 @@
         <v>13</v>
       </c>
       <c r="B109" s="14">
-        <f>1/4</f>
-        <v>0.25</v>
+        <f>COUNTIF(B111:B114, "+")/COUNTA(B111:B114)</f>
+        <v>0.5</v>
       </c>
       <c r="C109" s="11"/>
       <c r="D109" s="14">
@@ -1676,19 +1723,27 @@
       <c r="A112" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="B112" t="s">
+        <v>88</v>
+      </c>
       <c r="E112" s="4"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>84</v>
       </c>
+      <c r="B113" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B114" s="6"/>
+      <c r="B114" s="16" t="s">
+        <v>94</v>
+      </c>
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
       <c r="E114" s="7"/>

</xml_diff>

<commit_message>
Add running in parallel
</commit_message>
<xml_diff>
--- a/WhatTheShop_progress.xlsx
+++ b/WhatTheShop_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\whattheshop-fetcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE849FFE-3B4B-4CF4-BBA9-3992F464C3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E01F55-7ACB-47B7-8C2A-C2D8E50E2B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{A165CAB8-4234-4E81-A305-F753D69B9A3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="99">
   <si>
     <t>User</t>
   </si>
@@ -311,16 +311,28 @@
     <t>bad api</t>
   </si>
   <si>
-    <t>72 endpoints</t>
-  </si>
-  <si>
     <t>return empty</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>// it requires sensor or hardware id. It's not available in the API</t>
+  </si>
+  <si>
+    <t>Total endpoints</t>
+  </si>
+  <si>
+    <t>API handled</t>
+  </si>
+  <si>
+    <t>API Handled</t>
+  </si>
+  <si>
+    <t>API to DB done</t>
+  </si>
+  <si>
+    <t>Excel filler</t>
+  </si>
+  <si>
+    <t>Always empty</t>
   </si>
 </sst>
 </file>
@@ -359,7 +371,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -471,10 +483,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -488,9 +512,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -498,10 +520,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="2"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="11" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Total" xfId="2" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -813,61 +838,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D883A3CC-69E9-4B5D-8D31-B2725BBDF0A5}">
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="3" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="9">
-        <f>AVERAGE(B3,B10,B20,B26,B40,B51,B62,B74,B80,B88,B92,B99,B104,B109)</f>
-        <v>0.73726551226551218</v>
+      <c r="C1" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="10">
-        <f>AVERAGE(D3,D10,D20,D26,D40,D51,D62,D74,D80,D88,D92,D99,D104,D109)</f>
-        <v>0.10204081632653061</v>
-      </c>
-      <c r="G1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E1" s="10"/>
+      <c r="G1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="15">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="12">
+        <f>COUNTIF(B4:B8, "+")/ROWS(B4:B8)</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="12">
+        <f>COUNTA(B4:B8)/ROWS(B4:B8)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="12">
+        <f>COUNTIF(D4:D8, "+")/ROWS(D4:D8)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="G2" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="16">
+        <f>SUM(B2,B10,B20,B26,B40,B51,B62,B74,B80,B88,B92,B99,B104,B109)/14</f>
+        <v>0.6980132962275819</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
-      <c r="B3" s="3">
-        <f>5/5</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <f>4/4</f>
-        <v>1</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="16">
+        <f>SUM(C2,C10,C20,C26,C40,C51,C62,C74,C80,C88,C92,C99,C104,C109)/14</f>
+        <v>0.8660714285714286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -875,11 +915,20 @@
         <v>88</v>
       </c>
       <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="16">
+        <f>SUM(D2,D10,D20,D26,D40,D51,D62,D74,D80,D88,D92,D99,D104,D109)/14</f>
+        <v>0.10204081632653061</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -891,7 +940,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -903,7 +952,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -915,7 +964,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
@@ -928,27 +977,30 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="13">
-        <f>4/7</f>
+      <c r="B10" s="12">
+        <f>COUNTIF(B12:B18, "+")/ROWS(B12:B18)</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="13">
-        <f>3/7</f>
+      <c r="C10" s="12">
+        <f>COUNTA(B12:B18)/ROWS(B12:B18)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="12">
+        <f>COUNTIF(D12:D18, "+")/ROWS(D12:D18)</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -960,7 +1012,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -972,7 +1024,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -984,7 +1036,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -993,7 +1045,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -1027,16 +1079,19 @@
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="13">
-        <f>3/3</f>
-        <v>1</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="13">
-        <f>0/3</f>
+      <c r="B20" s="12">
+        <f>COUNTIF(B22:B24, "+")/ROWS(B22:B24)</f>
+        <v>1</v>
+      </c>
+      <c r="C20" s="12">
+        <f>COUNTA(B22:B24)/ROWS(B22:B24)</f>
+        <v>1</v>
+      </c>
+      <c r="D20" s="12">
+        <f>COUNTIF(D22:D24, "+")/ROWS(D22:D24)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
@@ -1076,16 +1131,19 @@
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="13">
-        <f>10/11</f>
+      <c r="B26" s="12">
+        <f>COUNTIF(B28:B38, "+")/ROWS(B28:B38)</f>
         <v>0.90909090909090906</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="13">
-        <f>0/11</f>
+      <c r="C26" s="12">
+        <f>COUNTA(B28:B38)/ROWS(B28:B38)</f>
+        <v>1</v>
+      </c>
+      <c r="D26" s="12">
+        <f>COUNTIF(D28:D38, "+")/ROWS(D28:D38)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
@@ -1197,16 +1255,19 @@
       <c r="A40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="14">
-        <f>0/8</f>
+      <c r="B40" s="12">
+        <f>COUNTIF(B42:B49, "+")/ROWS(B42:B49)</f>
+        <v>1</v>
+      </c>
+      <c r="C40" s="12">
+        <f>COUNTA(B42:B49)/ROWS(B42:B49)</f>
+        <v>1</v>
+      </c>
+      <c r="D40" s="12">
+        <f>COUNTIF(D42:D49, "+")/ROWS(D42:D49)</f>
         <v>0</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="14">
-        <f>0/8</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="12"/>
+      <c r="E40" s="11"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
@@ -1216,49 +1277,72 @@
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
       <c r="E43" s="4"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
       <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
       <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
       <c r="E46" s="4"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
       <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="B48" t="s">
+        <v>88</v>
+      </c>
       <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="6"/>
+      <c r="B49" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="7"/>
@@ -1268,13 +1352,19 @@
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="14"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="14">
-        <f>0/8</f>
+      <c r="B51" s="12">
+        <f>COUNTIF(B53:B60, "+")/ROWS(B53:B60)</f>
+        <v>0.125</v>
+      </c>
+      <c r="C51" s="12">
+        <f>COUNTA(B53:B60)/ROWS(B53:B60)</f>
+        <v>0.125</v>
+      </c>
+      <c r="D51" s="12">
+        <f>COUNTIF(D53:D60, "+")/ROWS(D53:D60)</f>
         <v>0</v>
       </c>
-      <c r="E51" s="12"/>
+      <c r="E51" s="11"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
@@ -1283,6 +1373,9 @@
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>48</v>
+      </c>
+      <c r="B53" t="s">
+        <v>88</v>
       </c>
       <c r="E53" s="4"/>
     </row>
@@ -1336,13 +1429,19 @@
       <c r="A62" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="14">
-        <f>0/9</f>
+      <c r="B62" s="12">
+        <f>COUNTIF(B64:B72, "+")/ROWS(B64:B72)</f>
         <v>0</v>
       </c>
-      <c r="E62" s="12"/>
+      <c r="C62" s="12">
+        <f>COUNTA(B64:B72)/ROWS(B64:B72)</f>
+        <v>0</v>
+      </c>
+      <c r="D62" s="12">
+        <f>COUNTIF(D64:D72, "+")/ROWS(D64:D72)</f>
+        <v>0</v>
+      </c>
+      <c r="E62" s="11"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
@@ -1410,16 +1509,19 @@
       <c r="A74" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B74" s="14">
-        <f>COUNTIF(B76:B78, "+")/COUNTA(B76:B78)</f>
+      <c r="B74" s="12">
+        <f>COUNTIF(B76:B78, "+")/ROWS(B76:B78)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C74" s="11"/>
-      <c r="D74" s="14">
-        <f>0/3</f>
+      <c r="C74" s="12">
+        <f>COUNTA(B76:B78)/ROWS(B76:B78)</f>
+        <v>1</v>
+      </c>
+      <c r="D74" s="12">
+        <f>COUNTIF(D76:D78, "+")/ROWS(D76:D78)</f>
         <v>0</v>
       </c>
-      <c r="E74" s="12"/>
+      <c r="E74" s="11"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
@@ -1448,7 +1550,7 @@
         <v>67</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
@@ -1459,16 +1561,19 @@
       <c r="A80" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B80" s="14">
-        <f>COUNTIF(B82:B86, "+")/COUNTA(B82:B86)</f>
-        <v>0.2</v>
-      </c>
-      <c r="C80" s="11"/>
-      <c r="D80" s="14">
-        <f>0/5</f>
+      <c r="B80" s="12">
+        <f>COUNTIF(B82:B86, "+")/ROWS(B82:B86)</f>
+        <v>1</v>
+      </c>
+      <c r="C80" s="12">
+        <f>COUNTA(B82:B86)/ROWS(B82:B86)</f>
+        <v>1</v>
+      </c>
+      <c r="D80" s="12">
+        <f>COUNTIF(D82:D86, "+")/ROWS(D82:D86)</f>
         <v>0</v>
       </c>
-      <c r="E80" s="12"/>
+      <c r="E80" s="11"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
@@ -1488,7 +1593,7 @@
         <v>69</v>
       </c>
       <c r="B83" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E83" s="4"/>
     </row>
@@ -1497,7 +1602,7 @@
         <v>70</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E84" s="4"/>
     </row>
@@ -1506,7 +1611,7 @@
         <v>71</v>
       </c>
       <c r="B85" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E85" s="4"/>
     </row>
@@ -1515,7 +1620,7 @@
         <v>72</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
@@ -1526,16 +1631,19 @@
       <c r="A88" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B88" s="14">
-        <f>COUNTIF(B90, "+")/COUNTA(B90)</f>
-        <v>1</v>
-      </c>
-      <c r="C88" s="11"/>
-      <c r="D88" s="14">
-        <f>0/1</f>
+      <c r="B88" s="12">
+        <f>COUNTIF(B90:B90, "+")/ROWS(B90:B90)</f>
+        <v>1</v>
+      </c>
+      <c r="C88" s="12">
+        <f>COUNTA(B90:B90)/ROWS(B90:B90)</f>
+        <v>1</v>
+      </c>
+      <c r="D88" s="12">
+        <f>COUNTIF(D90:D90, "+")/ROWS(D90:D90)</f>
         <v>0</v>
       </c>
-      <c r="E88" s="12"/>
+      <c r="E88" s="11"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
@@ -1557,16 +1665,19 @@
       <c r="A92" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B92" s="14">
-        <f>COUNTIF(B94:B97, "+")/COUNTA(B94:B97)</f>
-        <v>1</v>
-      </c>
-      <c r="C92" s="11"/>
-      <c r="D92" s="14">
-        <f>0/4</f>
+      <c r="B92" s="12">
+        <f>COUNTIF(B94:B97, "+")/ROWS(B94:B97)</f>
+        <v>1</v>
+      </c>
+      <c r="C92" s="12">
+        <f>COUNTA(B94:B97)/ROWS(B94:B97)</f>
+        <v>1</v>
+      </c>
+      <c r="D92" s="12">
+        <f>COUNTIF(D94:D97, "+")/ROWS(D94:D97)</f>
         <v>0</v>
       </c>
-      <c r="E92" s="12"/>
+      <c r="E92" s="11"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
@@ -1615,16 +1726,19 @@
       <c r="A99" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B99" s="14">
-        <f>COUNTIF(B101:B102, "+")/COUNTA(B101:B102)</f>
-        <v>1</v>
-      </c>
-      <c r="C99" s="11"/>
-      <c r="D99" s="14">
-        <f>0/5</f>
+      <c r="B99" s="12">
+        <f>COUNTIF(B101:B102, "+")/ROWS(B101:B102)</f>
+        <v>1</v>
+      </c>
+      <c r="C99" s="12">
+        <f>COUNTA(B101:B102)/ROWS(B101:B102)</f>
+        <v>1</v>
+      </c>
+      <c r="D99" s="12">
+        <f>COUNTIF(D101:D102, "+")/ROWS(D101:D102)</f>
         <v>0</v>
       </c>
-      <c r="E99" s="12"/>
+      <c r="E99" s="11"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
@@ -1655,16 +1769,19 @@
       <c r="A104" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B104" s="14">
-        <f>2/2</f>
-        <v>1</v>
-      </c>
-      <c r="C104" s="11"/>
-      <c r="D104" s="14">
-        <f>0/2</f>
+      <c r="B104" s="12">
+        <f>COUNTIF(B106:B107, "+")/ROWS(B106:B107)</f>
         <v>0</v>
       </c>
-      <c r="E104" s="12"/>
+      <c r="C104" s="12">
+        <f>COUNTA(B106:B107)/ROWS(B106:B107)</f>
+        <v>1</v>
+      </c>
+      <c r="D104" s="12">
+        <f>COUNTIF(D106:D107, "+")/ROWS(D106:D107)</f>
+        <v>0</v>
+      </c>
+      <c r="E104" s="11"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
@@ -1675,7 +1792,7 @@
         <v>80</v>
       </c>
       <c r="B106" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E106" s="4"/>
     </row>
@@ -1683,8 +1800,8 @@
       <c r="A107" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B107" s="6" t="s">
-        <v>88</v>
+      <c r="B107" t="s">
+        <v>98</v>
       </c>
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
@@ -1695,16 +1812,19 @@
       <c r="A109" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B109" s="14">
-        <f>COUNTIF(B111:B114, "+")/COUNTA(B111:B114)</f>
+      <c r="B109" s="12">
+        <f>COUNTIF(B111:B114, "+")/ROWS(B111:B114)</f>
         <v>0.5</v>
       </c>
-      <c r="C109" s="11"/>
-      <c r="D109" s="14">
-        <f>0/4</f>
+      <c r="C109" s="12">
+        <f>COUNTA(B111:B114)/ROWS(B111:B114)</f>
+        <v>1</v>
+      </c>
+      <c r="D109" s="12">
+        <f>COUNTIF(D111:D114, "+")/ROWS(D111:D114)</f>
         <v>0</v>
       </c>
-      <c r="E109" s="12"/>
+      <c r="E109" s="11"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
@@ -1732,8 +1852,8 @@
       <c r="A113" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B113" s="15" t="s">
-        <v>94</v>
+      <c r="B113" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="E113" s="4"/>
     </row>
@@ -1741,8 +1861,8 @@
       <c r="A114" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B114" s="16" t="s">
-        <v>94</v>
+      <c r="B114" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>

</xml_diff>